<commit_message>
Termino el proyecto, depurado y optimizado
</commit_message>
<xml_diff>
--- a/datos/depurando.xlsx
+++ b/datos/depurando.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">diego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alberto</t>
   </si>
 </sst>
 </file>
@@ -241,10 +244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,6 +283,25 @@
       </c>
       <c r="C3" s="1" t="n">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>